<commit_message>
fixed legends and tables
</commit_message>
<xml_diff>
--- a/results/supplement/tables/Table_S2.xlsx
+++ b/results/supplement/tables/Table_S2.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Normalized cDNA Reads and Annotation" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -12940,6 +12940,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -13012,22 +13013,22 @@
   </sheetPr>
   <dimension ref="A1:J1111"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.27040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.5357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="121.275510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="319.198979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="139.030612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.6173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="119.872448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="315.612244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="137.423469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>